<commit_message>
A few bugfixes and fixed tests. Added ResultNumeric property to Operator to handle blank rows and when comparing cell values
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/chainname.xlsx
+++ b/EPPlusTest/Workbooks/chainname.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevExternal\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Name">Sheet1!$B$8</definedName>
+    <definedName name="Name">Sheet1!$C$1</definedName>
     <definedName name="NameName">Name+Sheet1!$D$5</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -340,10 +340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -362,8 +362,8 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <f>SUM(B1:B6)</f>
-        <v>50</v>
+        <f>SUM(A1:A7)+C2</f>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -373,6 +373,10 @@
       <c r="B2">
         <f>A2+B1</f>
         <v>3</v>
+      </c>
+      <c r="C2">
+        <f>SUM(B1:B6)</f>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -414,14 +418,8 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>C1+B5</f>
+        <f>C2+B5</f>
         <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <f>SUM(A1:A7)+C1</f>
-        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>